<commit_message>
sprint 2 & 3
</commit_message>
<xml_diff>
--- a/teacher/assessment.xlsx
+++ b/teacher/assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h02680\Documents\software-development-project-1\teacher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68CFCEA-3A6A-4C53-9318-126781247EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BF0F35-768F-4F88-96FF-BDFCC290170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{F3B1C888-A306-445B-925E-DC4F729ADDF2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Team name</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>All documentation done and up-to-date</t>
+  </si>
+  <si>
+    <t>User story 8 implemented</t>
+  </si>
+  <si>
+    <t>Backlog has user story 8 tasks</t>
   </si>
 </sst>
 </file>
@@ -722,10 +728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2225FF66-A0D7-41EE-81D9-EFEBD5AB9F52}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1031,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1042,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1053,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1064,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1075,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1086,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1097,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1108,23 +1114,23 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1135,29 +1141,29 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1168,29 +1174,29 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1201,7 +1207,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1212,7 +1218,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1223,18 +1229,18 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1245,7 +1251,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1256,29 +1262,29 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1288,64 +1294,64 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3">
-        <f>SUM(C28:C51)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="3">
-        <f>SUM(D28:D51)</f>
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3">
+        <f>SUM(C28:C53)</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <f>SUM(D28:D53)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0.25</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1356,7 +1362,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1367,7 +1373,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1378,7 +1384,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1389,7 +1395,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1400,51 +1406,51 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1455,76 +1461,123 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>49</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3">
-        <f>SUM(C56:C73)</f>
-        <v>0</v>
-      </c>
-      <c r="D74" s="3">
-        <f>SUM(D56:D73)</f>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3">
+        <f>SUM(C58:C77)</f>
+        <v>0</v>
+      </c>
+      <c r="D78" s="3">
+        <f>SUM(D58:D77)</f>
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sprint 1 & 2
</commit_message>
<xml_diff>
--- a/teacher/assessment.xlsx
+++ b/teacher/assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h02680\Documents\software-development-project-1\teacher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BF0F35-768F-4F88-96FF-BDFCC290170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADC847E-5DBC-47F9-8259-55FCE1C1EAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{F3B1C888-A306-445B-925E-DC4F729ADDF2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
   <si>
     <t>Team name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Backlog has user story 8 tasks</t>
+  </si>
+  <si>
+    <t>Test database configuration</t>
   </si>
 </sst>
 </file>
@@ -728,10 +731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2225FF66-A0D7-41EE-81D9-EFEBD5AB9F52}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="95" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,7 +1409,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1417,7 +1420,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1428,24 +1431,24 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -1467,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1478,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -1489,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -1500,23 +1503,23 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1527,57 +1530,46 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>49</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3">
-        <f>SUM(C58:C77)</f>
-        <v>0</v>
-      </c>
-      <c r="D78" s="3">
-        <f>SUM(D58:D77)</f>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3">
+        <f>SUM(C58:C76)</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="3">
+        <f>SUM(D58:D76)</f>
         <v>10</v>
       </c>
     </row>

</xml_diff>